<commit_message>
sensor bill of material
</commit_message>
<xml_diff>
--- a/Production/BOMAnalogSensor_wk5.xlsx
+++ b/Production/BOMAnalogSensor_wk5.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mason\Downloads\eee3088f-project\Production\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sthab\Documents\EEE3088F\EEE3088F Project\Production\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD2C8125-C503-4414-916E-2BA10931BEB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881A77F4-4681-4CF6-A8F5-DE30C24A277A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{94F3FB38-0771-41C7-9436-2F9666787214}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{94F3FB38-0771-41C7-9436-2F9666787214}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -163,7 +161,7 @@
     <t xml:space="preserve">Total </t>
   </si>
   <si>
-    <t>$0.4043</t>
+    <t>$0.4067</t>
   </si>
 </sst>
 </file>
@@ -518,12 +516,18 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.36328125" customWidth="1"/>
+    <col min="2" max="2" width="19.08984375" customWidth="1"/>
+    <col min="3" max="3" width="7.36328125" customWidth="1"/>
+    <col min="4" max="4" width="46.453125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -549,7 +553,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -572,7 +576,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -598,7 +602,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -624,7 +628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -647,10 +651,10 @@
         <v>26</v>
       </c>
       <c r="H5">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -676,7 +680,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>41</v>
       </c>

</xml_diff>